<commit_message>
Finland NUTS3 to NUTS2
</commit_message>
<xml_diff>
--- a/data-raw/code_regions.xlsx
+++ b/data-raw/code_regions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/_package/eurobarometer/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Antal\OneDrive - Visegrad Investments\_package\eurobarometer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="363" documentId="8_{D45FB881-C323-449C-A41B-3807A3A86BF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{69E4234F-2E3D-45E6-A4AA-1BEC1DE67EF1}"/>
+  <xr:revisionPtr revIDLastSave="372" documentId="8_{D45FB881-C323-449C-A41B-3807A3A86BF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{BC62584B-4965-4664-AA68-B22727939707}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="847">
   <si>
     <t>country_code</t>
   </si>
@@ -2516,130 +2516,58 @@
     <t>Kainuu</t>
   </si>
   <si>
-    <t>NUTS level 4</t>
-  </si>
-  <si>
-    <t>NUTS level 5</t>
-  </si>
-  <si>
-    <t>FI1B1</t>
-  </si>
-  <si>
-    <t>NUTS level 6</t>
-  </si>
-  <si>
-    <t>NUTS level 7</t>
-  </si>
-  <si>
     <t>Varsinais-Suomi</t>
   </si>
   <si>
     <t>FI1C1</t>
   </si>
   <si>
-    <t>NUTS level 8</t>
-  </si>
-  <si>
-    <t>Kanta-Häme</t>
-  </si>
-  <si>
-    <t>FI1C2</t>
-  </si>
-  <si>
-    <t>NUTS level 9</t>
-  </si>
-  <si>
     <t>Päijät-Häme</t>
   </si>
   <si>
     <t>FI1C3</t>
   </si>
   <si>
-    <t>NUTS level 10</t>
-  </si>
-  <si>
     <t>FI1C4</t>
   </si>
   <si>
-    <t>NUTS level 11</t>
-  </si>
-  <si>
     <t>Etelä-Karjala</t>
   </si>
   <si>
     <t>FI1C5</t>
   </si>
   <si>
-    <t>NUTS level 12</t>
-  </si>
-  <si>
-    <t>NUTS level 13</t>
-  </si>
-  <si>
     <t>Etelä-Savo</t>
   </si>
   <si>
     <t>FI1D1</t>
   </si>
   <si>
-    <t>NUTS level 14</t>
-  </si>
-  <si>
     <t>Pohjois-Savo</t>
   </si>
   <si>
     <t>FI1D2</t>
   </si>
   <si>
-    <t>NUTS level 15</t>
-  </si>
-  <si>
     <t>Pohjois-Karjala</t>
   </si>
   <si>
     <t>FI1D3</t>
   </si>
   <si>
-    <t>NUTS level 16</t>
-  </si>
-  <si>
     <t>FI1D4</t>
   </si>
   <si>
-    <t>NUTS level 17</t>
-  </si>
-  <si>
     <t>Keski-Pohjanmaa</t>
   </si>
   <si>
     <t>FI1D5</t>
   </si>
   <si>
-    <t>NUTS level 18</t>
-  </si>
-  <si>
     <t>Pohjois-Pohjanmaa</t>
   </si>
   <si>
     <t>FI1D6</t>
-  </si>
-  <si>
-    <t>NUTS level 19</t>
-  </si>
-  <si>
-    <t>Lappi</t>
-  </si>
-  <si>
-    <t>FI1D7</t>
-  </si>
-  <si>
-    <t>NUTS level 20</t>
-  </si>
-  <si>
-    <t>Åland</t>
-  </si>
-  <si>
-    <t>FI200</t>
   </si>
   <si>
     <t>Ditiki Ellada</t>
@@ -3561,10 +3489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J302"/>
+  <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="A285" sqref="A285:XFD285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5759,7 +5687,7 @@
         <v>802</v>
       </c>
       <c r="B96" t="s">
-        <v>869</v>
+        <v>845</v>
       </c>
       <c r="C96" t="s">
         <v>9</v>
@@ -5939,7 +5867,7 @@
         <v>802</v>
       </c>
       <c r="B105" t="s">
-        <v>870</v>
+        <v>846</v>
       </c>
       <c r="C105" t="s">
         <v>9</v>
@@ -9920,24 +9848,30 @@
       <c r="A280" t="s">
         <v>101</v>
       </c>
+      <c r="B280" t="s">
+        <v>803</v>
+      </c>
       <c r="C280" t="s">
         <v>638</v>
       </c>
       <c r="E280">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="F280" t="str">
-        <f>LEFT(I280,4)</f>
+        <f t="shared" ref="F280:F294" si="0">LEFT(I280,4)</f>
         <v>FI19</v>
       </c>
       <c r="G280" t="s">
         <v>591</v>
       </c>
+      <c r="H280" t="s">
+        <v>804</v>
+      </c>
       <c r="I280" t="s">
-        <v>590</v>
+        <v>809</v>
       </c>
       <c r="J280" t="s">
-        <v>590</v>
+        <v>809</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.25">
@@ -9945,29 +9879,29 @@
         <v>101</v>
       </c>
       <c r="B281" t="s">
-        <v>803</v>
+        <v>820</v>
       </c>
       <c r="C281" t="s">
         <v>638</v>
       </c>
       <c r="E281">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="F281" t="str">
-        <f t="shared" ref="F281:F302" si="0">LEFT(I281,4)</f>
+        <f t="shared" si="0"/>
         <v>FI19</v>
       </c>
       <c r="G281" t="s">
         <v>591</v>
       </c>
       <c r="H281" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="I281" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="J281" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.25">
@@ -9975,13 +9909,13 @@
         <v>101</v>
       </c>
       <c r="B282" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="C282" t="s">
         <v>638</v>
       </c>
       <c r="E282">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="F282" t="str">
         <f t="shared" si="0"/>
@@ -9991,13 +9925,13 @@
         <v>591</v>
       </c>
       <c r="H282" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="I282" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="J282" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
@@ -10005,13 +9939,13 @@
         <v>101</v>
       </c>
       <c r="B283" t="s">
-        <v>823</v>
+        <v>807</v>
       </c>
       <c r="C283" t="s">
         <v>638</v>
       </c>
       <c r="E283">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="F283" t="str">
         <f t="shared" si="0"/>
@@ -10021,13 +9955,13 @@
         <v>591</v>
       </c>
       <c r="H283" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="I283" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="J283" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.25">
@@ -10035,13 +9969,13 @@
         <v>101</v>
       </c>
       <c r="B284" t="s">
-        <v>807</v>
+        <v>815</v>
       </c>
       <c r="C284" t="s">
         <v>638</v>
       </c>
       <c r="E284">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="F284" t="str">
         <f t="shared" si="0"/>
@@ -10051,13 +9985,13 @@
         <v>591</v>
       </c>
       <c r="H284" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="I284" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="J284" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.25">
@@ -10065,53 +9999,59 @@
         <v>101</v>
       </c>
       <c r="B285" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c r="C285" t="s">
         <v>638</v>
       </c>
       <c r="E285">
-        <v>1613</v>
+        <v>1617</v>
       </c>
       <c r="F285" t="str">
         <f t="shared" si="0"/>
-        <v>FI19</v>
+        <v>FI1C</v>
       </c>
       <c r="G285" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="H285" t="s">
-        <v>808</v>
+        <v>827</v>
       </c>
       <c r="I285" t="s">
-        <v>813</v>
+        <v>828</v>
       </c>
       <c r="J285" t="s">
-        <v>813</v>
+        <v>828</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>101</v>
       </c>
+      <c r="B286" t="s">
+        <v>824</v>
+      </c>
       <c r="C286" t="s">
-        <v>827</v>
+        <v>638</v>
       </c>
       <c r="E286">
-        <v>1614</v>
+        <v>1619</v>
       </c>
       <c r="F286" t="str">
         <f t="shared" si="0"/>
-        <v>FI1B</v>
+        <v>FI1C</v>
       </c>
       <c r="G286" t="s">
-        <v>102</v>
+        <v>594</v>
+      </c>
+      <c r="H286" t="s">
+        <v>829</v>
       </c>
       <c r="I286" t="s">
-        <v>104</v>
+        <v>830</v>
       </c>
       <c r="J286" t="s">
-        <v>104</v>
+        <v>830</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
@@ -10119,40 +10059,43 @@
         <v>101</v>
       </c>
       <c r="B287" t="s">
-        <v>102</v>
+        <v>817</v>
       </c>
       <c r="C287" t="s">
-        <v>828</v>
+        <v>638</v>
       </c>
       <c r="E287">
-        <v>1615</v>
+        <v>1620</v>
       </c>
       <c r="F287" t="str">
         <f t="shared" si="0"/>
-        <v>FI1B</v>
+        <v>FI1C</v>
       </c>
       <c r="G287" t="s">
-        <v>102</v>
+        <v>594</v>
       </c>
       <c r="H287" t="s">
-        <v>102</v>
+        <v>817</v>
       </c>
       <c r="I287" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="J287" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>101</v>
       </c>
+      <c r="B288" t="s">
+        <v>825</v>
+      </c>
       <c r="C288" t="s">
-        <v>830</v>
+        <v>638</v>
       </c>
       <c r="E288">
-        <v>1616</v>
+        <v>1621</v>
       </c>
       <c r="F288" t="str">
         <f t="shared" si="0"/>
@@ -10161,11 +10104,14 @@
       <c r="G288" t="s">
         <v>594</v>
       </c>
+      <c r="H288" t="s">
+        <v>832</v>
+      </c>
       <c r="I288" t="s">
-        <v>593</v>
+        <v>833</v>
       </c>
       <c r="J288" t="s">
-        <v>593</v>
+        <v>833</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
@@ -10173,56 +10119,59 @@
         <v>101</v>
       </c>
       <c r="B289" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="C289" t="s">
-        <v>831</v>
+        <v>638</v>
       </c>
       <c r="E289">
-        <v>1617</v>
+        <v>1623</v>
       </c>
       <c r="F289" t="str">
         <f t="shared" si="0"/>
-        <v>FI1C</v>
+        <v>FI1D</v>
       </c>
       <c r="G289" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="H289" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="I289" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="J289" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>101</v>
       </c>
+      <c r="B290" t="s">
+        <v>821</v>
+      </c>
       <c r="C290" t="s">
-        <v>834</v>
+        <v>638</v>
       </c>
       <c r="E290">
-        <v>1618</v>
+        <v>1624</v>
       </c>
       <c r="F290" t="str">
         <f t="shared" si="0"/>
-        <v>FI1C</v>
+        <v>FI1D</v>
       </c>
       <c r="G290" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="H290" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="I290" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="J290" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.25">
@@ -10230,20 +10179,20 @@
         <v>101</v>
       </c>
       <c r="B291" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="C291" t="s">
-        <v>837</v>
+        <v>638</v>
       </c>
       <c r="E291">
-        <v>1619</v>
+        <v>1625</v>
       </c>
       <c r="F291" t="str">
         <f t="shared" si="0"/>
-        <v>FI1C</v>
+        <v>FI1D</v>
       </c>
       <c r="G291" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="H291" t="s">
         <v>838</v>
@@ -10260,29 +10209,29 @@
         <v>101</v>
       </c>
       <c r="B292" t="s">
-        <v>817</v>
+        <v>826</v>
       </c>
       <c r="C292" t="s">
-        <v>840</v>
+        <v>638</v>
       </c>
       <c r="E292">
-        <v>1620</v>
+        <v>1626</v>
       </c>
       <c r="F292" t="str">
         <f t="shared" si="0"/>
-        <v>FI1C</v>
+        <v>FI1D</v>
       </c>
       <c r="G292" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="H292" t="s">
-        <v>817</v>
+        <v>826</v>
       </c>
       <c r="I292" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="J292" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
@@ -10290,40 +10239,43 @@
         <v>101</v>
       </c>
       <c r="B293" t="s">
-        <v>825</v>
+        <v>814</v>
       </c>
       <c r="C293" t="s">
-        <v>842</v>
+        <v>638</v>
       </c>
       <c r="E293">
-        <v>1621</v>
+        <v>1627</v>
       </c>
       <c r="F293" t="str">
         <f t="shared" si="0"/>
-        <v>FI1C</v>
+        <v>FI1D</v>
       </c>
       <c r="G293" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="H293" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="I293" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="J293" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>101</v>
       </c>
+      <c r="B294" t="s">
+        <v>816</v>
+      </c>
       <c r="C294" t="s">
-        <v>845</v>
+        <v>638</v>
       </c>
       <c r="E294">
-        <v>1622</v>
+        <v>1628</v>
       </c>
       <c r="F294" t="str">
         <f t="shared" si="0"/>
@@ -10332,245 +10284,14 @@
       <c r="G294" t="s">
         <v>597</v>
       </c>
+      <c r="H294" t="s">
+        <v>843</v>
+      </c>
       <c r="I294" t="s">
-        <v>596</v>
+        <v>844</v>
       </c>
       <c r="J294" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
-        <v>101</v>
-      </c>
-      <c r="B295" t="s">
-        <v>822</v>
-      </c>
-      <c r="C295" t="s">
-        <v>846</v>
-      </c>
-      <c r="E295">
-        <v>1623</v>
-      </c>
-      <c r="F295" t="str">
-        <f t="shared" si="0"/>
-        <v>FI1D</v>
-      </c>
-      <c r="G295" t="s">
-        <v>597</v>
-      </c>
-      <c r="H295" t="s">
-        <v>847</v>
-      </c>
-      <c r="I295" t="s">
-        <v>848</v>
-      </c>
-      <c r="J295" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>101</v>
-      </c>
-      <c r="B296" t="s">
-        <v>821</v>
-      </c>
-      <c r="C296" t="s">
-        <v>849</v>
-      </c>
-      <c r="E296">
-        <v>1624</v>
-      </c>
-      <c r="F296" t="str">
-        <f t="shared" si="0"/>
-        <v>FI1D</v>
-      </c>
-      <c r="G296" t="s">
-        <v>597</v>
-      </c>
-      <c r="H296" t="s">
-        <v>850</v>
-      </c>
-      <c r="I296" t="s">
-        <v>851</v>
-      </c>
-      <c r="J296" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>101</v>
-      </c>
-      <c r="B297" t="s">
-        <v>818</v>
-      </c>
-      <c r="C297" t="s">
-        <v>852</v>
-      </c>
-      <c r="E297">
-        <v>1625</v>
-      </c>
-      <c r="F297" t="str">
-        <f t="shared" si="0"/>
-        <v>FI1D</v>
-      </c>
-      <c r="G297" t="s">
-        <v>597</v>
-      </c>
-      <c r="H297" t="s">
-        <v>853</v>
-      </c>
-      <c r="I297" t="s">
-        <v>854</v>
-      </c>
-      <c r="J297" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>101</v>
-      </c>
-      <c r="B298" t="s">
-        <v>826</v>
-      </c>
-      <c r="C298" t="s">
-        <v>855</v>
-      </c>
-      <c r="E298">
-        <v>1626</v>
-      </c>
-      <c r="F298" t="str">
-        <f t="shared" si="0"/>
-        <v>FI1D</v>
-      </c>
-      <c r="G298" t="s">
-        <v>597</v>
-      </c>
-      <c r="H298" t="s">
-        <v>826</v>
-      </c>
-      <c r="I298" t="s">
-        <v>856</v>
-      </c>
-      <c r="J298" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>101</v>
-      </c>
-      <c r="B299" t="s">
-        <v>814</v>
-      </c>
-      <c r="C299" t="s">
-        <v>857</v>
-      </c>
-      <c r="E299">
-        <v>1627</v>
-      </c>
-      <c r="F299" t="str">
-        <f t="shared" si="0"/>
-        <v>FI1D</v>
-      </c>
-      <c r="G299" t="s">
-        <v>597</v>
-      </c>
-      <c r="H299" t="s">
-        <v>858</v>
-      </c>
-      <c r="I299" t="s">
-        <v>859</v>
-      </c>
-      <c r="J299" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>101</v>
-      </c>
-      <c r="B300" t="s">
-        <v>816</v>
-      </c>
-      <c r="C300" t="s">
-        <v>860</v>
-      </c>
-      <c r="E300">
-        <v>1628</v>
-      </c>
-      <c r="F300" t="str">
-        <f t="shared" si="0"/>
-        <v>FI1D</v>
-      </c>
-      <c r="G300" t="s">
-        <v>597</v>
-      </c>
-      <c r="H300" t="s">
-        <v>861</v>
-      </c>
-      <c r="I300" t="s">
-        <v>862</v>
-      </c>
-      <c r="J300" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>101</v>
-      </c>
-      <c r="C301" t="s">
-        <v>863</v>
-      </c>
-      <c r="E301">
-        <v>1629</v>
-      </c>
-      <c r="F301" t="str">
-        <f t="shared" si="0"/>
-        <v>FI1D</v>
-      </c>
-      <c r="G301" t="s">
-        <v>597</v>
-      </c>
-      <c r="H301" t="s">
-        <v>864</v>
-      </c>
-      <c r="I301" t="s">
-        <v>865</v>
-      </c>
-      <c r="J301" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
-        <v>101</v>
-      </c>
-      <c r="C302" t="s">
-        <v>866</v>
-      </c>
-      <c r="E302">
-        <v>1632</v>
-      </c>
-      <c r="F302" t="str">
-        <f t="shared" si="0"/>
-        <v>FI20</v>
-      </c>
-      <c r="G302" t="s">
-        <v>867</v>
-      </c>
-      <c r="H302" t="s">
-        <v>867</v>
-      </c>
-      <c r="I302" t="s">
-        <v>868</v>
-      </c>
-      <c r="J302" t="s">
-        <v>868</v>
+        <v>844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code NUTS1 codes for DE, GB, IT plus CY, EE, LU, MT
</commit_message>
<xml_diff>
--- a/data-raw/code_regions.xlsx
+++ b/data-raw/code_regions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Antal\OneDrive - Visegrad Investments\_package\eurobarometer\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/_package/eurobarometer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="487" documentId="8_{D45FB881-C323-449C-A41B-3807A3A86BF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{D435AE56-5904-42CC-8AE7-AF28247DC25F}"/>
+  <xr:revisionPtr revIDLastSave="525" documentId="8_{D45FB881-C323-449C-A41B-3807A3A86BF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{6565C1C8-A342-45C5-B2DD-12C0455EAE89}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="small" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NUTS2!$A$1:$H$278</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NUTS2!$A$1:$H$293</definedName>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">Sheet2!$A$1:$L$131</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="1446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3556" uniqueCount="1444">
   <si>
     <t>country_code</t>
   </si>
@@ -4335,12 +4335,6 @@
   </si>
   <si>
     <t>1824</t>
-  </si>
-  <si>
-    <t>code_2010</t>
-  </si>
-  <si>
-    <t>code_2013</t>
   </si>
   <si>
     <t>Isole</t>
@@ -4758,7 +4752,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -4895,6 +4889,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4940,7 +4943,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4974,6 +4977,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5405,10 +5414,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B223" sqref="B223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5443,7 +5453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>193</v>
       </c>
@@ -5466,7 +5476,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -5489,7 +5499,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -5512,7 +5522,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>193</v>
       </c>
@@ -5535,7 +5545,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>193</v>
       </c>
@@ -5558,7 +5568,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>193</v>
       </c>
@@ -5581,7 +5591,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>193</v>
       </c>
@@ -5604,7 +5614,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>193</v>
       </c>
@@ -5627,7 +5637,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>193</v>
       </c>
@@ -5650,7 +5660,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>193</v>
       </c>
@@ -5673,7 +5683,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -5696,7 +5706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -5719,7 +5729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -5742,7 +5752,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -5765,7 +5775,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -5788,7 +5798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -5811,7 +5821,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -5834,7 +5844,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -5857,7 +5867,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -5880,7 +5890,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -5903,7 +5913,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -5926,7 +5936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>255</v>
       </c>
@@ -5949,7 +5959,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>255</v>
       </c>
@@ -5970,7 +5980,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>255</v>
       </c>
@@ -5993,7 +6003,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>255</v>
       </c>
@@ -6014,7 +6024,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>255</v>
       </c>
@@ -6037,7 +6047,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>255</v>
       </c>
@@ -6060,7 +6070,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>255</v>
       </c>
@@ -6086,7 +6096,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>255</v>
       </c>
@@ -6112,7 +6122,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>255</v>
       </c>
@@ -6138,7 +6148,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>255</v>
       </c>
@@ -6164,7 +6174,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>255</v>
       </c>
@@ -6190,7 +6200,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>255</v>
       </c>
@@ -6216,7 +6226,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>255</v>
       </c>
@@ -6242,7 +6252,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>255</v>
       </c>
@@ -6268,7 +6278,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>255</v>
       </c>
@@ -6294,7 +6304,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>255</v>
       </c>
@@ -6320,7 +6330,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>255</v>
       </c>
@@ -6346,7 +6356,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>255</v>
       </c>
@@ -6372,7 +6382,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>255</v>
       </c>
@@ -6398,7 +6408,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>255</v>
       </c>
@@ -6424,7 +6434,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>255</v>
       </c>
@@ -6450,7 +6460,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>255</v>
       </c>
@@ -6476,7 +6486,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>255</v>
       </c>
@@ -6502,7 +6512,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>255</v>
       </c>
@@ -6528,7 +6538,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>255</v>
       </c>
@@ -6554,7 +6564,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>255</v>
       </c>
@@ -6580,7 +6590,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>255</v>
       </c>
@@ -6606,7 +6616,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>255</v>
       </c>
@@ -6632,7 +6642,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>255</v>
       </c>
@@ -6658,7 +6668,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>255</v>
       </c>
@@ -6684,7 +6694,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>255</v>
       </c>
@@ -6710,7 +6720,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>255</v>
       </c>
@@ -6736,7 +6746,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>255</v>
       </c>
@@ -6762,7 +6772,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>255</v>
       </c>
@@ -6805,7 +6815,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>262</v>
       </c>
@@ -6828,7 +6838,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>262</v>
       </c>
@@ -6851,7 +6861,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>262</v>
       </c>
@@ -6874,7 +6884,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>262</v>
       </c>
@@ -6897,7 +6907,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -6920,7 +6930,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>262</v>
       </c>
@@ -6943,7 +6953,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>262</v>
       </c>
@@ -6966,7 +6976,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>262</v>
       </c>
@@ -6989,7 +6999,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>51</v>
       </c>
@@ -7012,7 +7022,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>51</v>
       </c>
@@ -7035,7 +7045,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>51</v>
       </c>
@@ -7058,7 +7068,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -7081,7 +7091,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>51</v>
       </c>
@@ -7242,7 +7252,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -7265,7 +7275,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -7288,7 +7298,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>75</v>
       </c>
@@ -7311,7 +7321,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>75</v>
       </c>
@@ -7334,7 +7344,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>75</v>
       </c>
@@ -7357,7 +7367,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>75</v>
       </c>
@@ -7380,7 +7390,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>75</v>
       </c>
@@ -7403,7 +7413,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>75</v>
       </c>
@@ -7426,7 +7436,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>75</v>
       </c>
@@ -7449,7 +7459,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
@@ -7472,7 +7482,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>75</v>
       </c>
@@ -7495,7 +7505,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>75</v>
       </c>
@@ -7518,7 +7528,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>75</v>
       </c>
@@ -7541,7 +7551,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>75</v>
       </c>
@@ -7567,7 +7577,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>75</v>
       </c>
@@ -7590,7 +7600,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>75</v>
       </c>
@@ -7613,7 +7623,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>75</v>
       </c>
@@ -7636,7 +7646,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>75</v>
       </c>
@@ -7656,7 +7666,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>75</v>
       </c>
@@ -7679,7 +7689,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -7702,7 +7712,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -7725,7 +7735,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -7748,7 +7758,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -7771,7 +7781,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>101</v>
       </c>
@@ -7794,7 +7804,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -7817,7 +7827,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -7831,7 +7841,7 @@
         <v>1609</v>
       </c>
       <c r="F102" t="str">
-        <f>LEFT(I102,4)</f>
+        <f t="shared" ref="F102:F116" si="0">LEFT(I102,4)</f>
         <v>FI19</v>
       </c>
       <c r="G102" t="s">
@@ -7847,7 +7857,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -7861,7 +7871,7 @@
         <v>1610</v>
       </c>
       <c r="F103" t="str">
-        <f>LEFT(I103,4)</f>
+        <f t="shared" si="0"/>
         <v>FI19</v>
       </c>
       <c r="G103" t="s">
@@ -7877,7 +7887,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -7891,7 +7901,7 @@
         <v>1611</v>
       </c>
       <c r="F104" t="str">
-        <f>LEFT(I104,4)</f>
+        <f t="shared" si="0"/>
         <v>FI19</v>
       </c>
       <c r="G104" t="s">
@@ -7907,7 +7917,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>101</v>
       </c>
@@ -7921,7 +7931,7 @@
         <v>1612</v>
       </c>
       <c r="F105" t="str">
-        <f>LEFT(I105,4)</f>
+        <f t="shared" si="0"/>
         <v>FI19</v>
       </c>
       <c r="G105" t="s">
@@ -7937,7 +7947,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -7951,7 +7961,7 @@
         <v>1613</v>
       </c>
       <c r="F106" t="str">
-        <f>LEFT(I106,4)</f>
+        <f t="shared" si="0"/>
         <v>FI19</v>
       </c>
       <c r="G106" t="s">
@@ -7967,7 +7977,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>101</v>
       </c>
@@ -7981,7 +7991,7 @@
         <v>1617</v>
       </c>
       <c r="F107" t="str">
-        <f>LEFT(I107,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1C</v>
       </c>
       <c r="G107" t="s">
@@ -7997,7 +8007,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>101</v>
       </c>
@@ -8011,7 +8021,7 @@
         <v>1619</v>
       </c>
       <c r="F108" t="str">
-        <f>LEFT(I108,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1C</v>
       </c>
       <c r="G108" t="s">
@@ -8027,7 +8037,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>101</v>
       </c>
@@ -8041,7 +8051,7 @@
         <v>1620</v>
       </c>
       <c r="F109" t="str">
-        <f>LEFT(I109,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1C</v>
       </c>
       <c r="G109" t="s">
@@ -8057,7 +8067,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>101</v>
       </c>
@@ -8071,7 +8081,7 @@
         <v>1621</v>
       </c>
       <c r="F110" t="str">
-        <f>LEFT(I110,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1C</v>
       </c>
       <c r="G110" t="s">
@@ -8087,7 +8097,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -8101,7 +8111,7 @@
         <v>1623</v>
       </c>
       <c r="F111" t="str">
-        <f>LEFT(I111,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1D</v>
       </c>
       <c r="G111" t="s">
@@ -8117,7 +8127,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>101</v>
       </c>
@@ -8131,7 +8141,7 @@
         <v>1624</v>
       </c>
       <c r="F112" t="str">
-        <f>LEFT(I112,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1D</v>
       </c>
       <c r="G112" t="s">
@@ -8147,7 +8157,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>101</v>
       </c>
@@ -8161,7 +8171,7 @@
         <v>1625</v>
       </c>
       <c r="F113" t="str">
-        <f>LEFT(I113,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1D</v>
       </c>
       <c r="G113" t="s">
@@ -8177,7 +8187,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>101</v>
       </c>
@@ -8191,7 +8201,7 @@
         <v>1626</v>
       </c>
       <c r="F114" t="str">
-        <f>LEFT(I114,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1D</v>
       </c>
       <c r="G114" t="s">
@@ -8207,7 +8217,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>101</v>
       </c>
@@ -8221,7 +8231,7 @@
         <v>1627</v>
       </c>
       <c r="F115" t="str">
-        <f>LEFT(I115,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1D</v>
       </c>
       <c r="G115" t="s">
@@ -8237,7 +8247,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>101</v>
       </c>
@@ -8251,7 +8261,7 @@
         <v>1628</v>
       </c>
       <c r="F116" t="str">
-        <f>LEFT(I116,4)</f>
+        <f t="shared" si="0"/>
         <v>FI1D</v>
       </c>
       <c r="G116" t="s">
@@ -8267,7 +8277,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>108</v>
       </c>
@@ -8290,7 +8300,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>108</v>
       </c>
@@ -8313,7 +8323,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>108</v>
       </c>
@@ -8336,7 +8346,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>108</v>
       </c>
@@ -8359,7 +8369,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>108</v>
       </c>
@@ -8382,7 +8392,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>108</v>
       </c>
@@ -8405,7 +8415,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>108</v>
       </c>
@@ -8428,7 +8438,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>108</v>
       </c>
@@ -8451,7 +8461,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>108</v>
       </c>
@@ -8474,7 +8484,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>108</v>
       </c>
@@ -8497,7 +8507,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>108</v>
       </c>
@@ -8520,7 +8530,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>108</v>
       </c>
@@ -8543,7 +8553,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>108</v>
       </c>
@@ -8566,7 +8576,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>108</v>
       </c>
@@ -8589,7 +8599,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>108</v>
       </c>
@@ -8612,7 +8622,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>108</v>
       </c>
@@ -8635,7 +8645,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>108</v>
       </c>
@@ -8658,7 +8668,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>108</v>
       </c>
@@ -8681,7 +8691,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>108</v>
       </c>
@@ -8704,7 +8714,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>108</v>
       </c>
@@ -8727,7 +8737,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>108</v>
       </c>
@@ -8750,7 +8760,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>108</v>
       </c>
@@ -8773,7 +8783,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>108</v>
       </c>
@@ -8796,7 +8806,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>108</v>
       </c>
@@ -8819,7 +8829,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>108</v>
       </c>
@@ -8842,7 +8852,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>108</v>
       </c>
@@ -8865,7 +8875,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>108</v>
       </c>
@@ -8888,7 +8898,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>108</v>
       </c>
@@ -8908,7 +8918,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>108</v>
       </c>
@@ -8928,7 +8938,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>736</v>
       </c>
@@ -8948,7 +8958,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>802</v>
       </c>
@@ -8968,7 +8978,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>802</v>
       </c>
@@ -8988,7 +8998,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>802</v>
       </c>
@@ -9008,7 +9018,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>802</v>
       </c>
@@ -9028,7 +9038,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>802</v>
       </c>
@@ -9048,7 +9058,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>802</v>
       </c>
@@ -9068,7 +9078,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>802</v>
       </c>
@@ -9088,7 +9098,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>802</v>
       </c>
@@ -9108,7 +9118,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>802</v>
       </c>
@@ -9128,7 +9138,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>802</v>
       </c>
@@ -9148,7 +9158,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>802</v>
       </c>
@@ -9168,7 +9178,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>802</v>
       </c>
@@ -9188,7 +9198,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>478</v>
       </c>
@@ -9211,7 +9221,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>478</v>
       </c>
@@ -9234,7 +9244,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>478</v>
       </c>
@@ -9254,7 +9264,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>478</v>
       </c>
@@ -9274,7 +9284,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>478</v>
       </c>
@@ -9294,7 +9304,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>478</v>
       </c>
@@ -9314,7 +9324,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>478</v>
       </c>
@@ -9334,7 +9344,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>478</v>
       </c>
@@ -9354,7 +9364,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>478</v>
       </c>
@@ -9374,7 +9384,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>478</v>
       </c>
@@ -9394,7 +9404,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>478</v>
       </c>
@@ -9414,7 +9424,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>478</v>
       </c>
@@ -9434,7 +9444,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>478</v>
       </c>
@@ -9454,7 +9464,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>478</v>
       </c>
@@ -9474,7 +9484,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>478</v>
       </c>
@@ -9494,7 +9504,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>478</v>
       </c>
@@ -9514,7 +9524,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>478</v>
       </c>
@@ -9534,7 +9544,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>478</v>
       </c>
@@ -9554,7 +9564,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>478</v>
       </c>
@@ -9574,7 +9584,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>478</v>
       </c>
@@ -9594,7 +9604,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>478</v>
       </c>
@@ -9614,7 +9624,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>478</v>
       </c>
@@ -9634,7 +9644,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>478</v>
       </c>
@@ -9654,7 +9664,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>275</v>
       </c>
@@ -9677,7 +9687,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>275</v>
       </c>
@@ -9700,7 +9710,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>275</v>
       </c>
@@ -9723,7 +9733,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>275</v>
       </c>
@@ -9746,7 +9756,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>275</v>
       </c>
@@ -9769,7 +9779,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>275</v>
       </c>
@@ -9792,7 +9802,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>275</v>
       </c>
@@ -9815,7 +9825,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>275</v>
       </c>
@@ -9838,7 +9848,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>275</v>
       </c>
@@ -9861,7 +9871,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>275</v>
       </c>
@@ -9884,7 +9894,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>275</v>
       </c>
@@ -9907,7 +9917,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>275</v>
       </c>
@@ -9930,7 +9940,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>275</v>
       </c>
@@ -9953,7 +9963,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>275</v>
       </c>
@@ -9976,7 +9986,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>373</v>
       </c>
@@ -9999,7 +10009,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>373</v>
       </c>
@@ -10022,7 +10032,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>373</v>
       </c>
@@ -10045,7 +10055,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>373</v>
       </c>
@@ -10068,7 +10078,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>373</v>
       </c>
@@ -10094,7 +10104,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>373</v>
       </c>
@@ -10117,7 +10127,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>373</v>
       </c>
@@ -10140,7 +10150,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>373</v>
       </c>
@@ -10163,7 +10173,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>373</v>
       </c>
@@ -10186,7 +10196,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>373</v>
       </c>
@@ -10209,7 +10219,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>491</v>
       </c>
@@ -10232,7 +10242,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>491</v>
       </c>
@@ -10255,7 +10265,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>491</v>
       </c>
@@ -10278,7 +10288,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>491</v>
       </c>
@@ -10301,7 +10311,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>491</v>
       </c>
@@ -10324,7 +10334,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>491</v>
       </c>
@@ -10347,7 +10357,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>491</v>
       </c>
@@ -10370,7 +10380,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>491</v>
       </c>
@@ -10393,7 +10403,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>491</v>
       </c>
@@ -10416,7 +10426,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>491</v>
       </c>
@@ -10457,7 +10467,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>487</v>
       </c>
@@ -10480,7 +10490,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>487</v>
       </c>
@@ -10503,7 +10513,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>487</v>
       </c>
@@ -10526,7 +10536,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>487</v>
       </c>
@@ -10549,7 +10559,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>487</v>
       </c>
@@ -10572,7 +10582,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>487</v>
       </c>
@@ -10612,7 +10622,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>154</v>
       </c>
@@ -10635,7 +10645,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>154</v>
       </c>
@@ -10658,7 +10668,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>154</v>
       </c>
@@ -10681,7 +10691,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>154</v>
       </c>
@@ -10704,7 +10714,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>154</v>
       </c>
@@ -10727,7 +10737,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>154</v>
       </c>
@@ -10750,7 +10760,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>154</v>
       </c>
@@ -10773,7 +10783,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>154</v>
       </c>
@@ -10796,7 +10806,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>154</v>
       </c>
@@ -10819,7 +10829,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>154</v>
       </c>
@@ -10842,7 +10852,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>154</v>
       </c>
@@ -10865,7 +10875,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>154</v>
       </c>
@@ -10888,7 +10898,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>283</v>
       </c>
@@ -10911,7 +10921,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>283</v>
       </c>
@@ -10934,7 +10944,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>283</v>
       </c>
@@ -10957,7 +10967,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>283</v>
       </c>
@@ -10980,7 +10990,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>283</v>
       </c>
@@ -11003,7 +11013,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>283</v>
       </c>
@@ -11026,7 +11036,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>283</v>
       </c>
@@ -11049,7 +11059,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>283</v>
       </c>
@@ -11072,7 +11082,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>283</v>
       </c>
@@ -11095,7 +11105,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>283</v>
       </c>
@@ -11118,7 +11128,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>283</v>
       </c>
@@ -11141,7 +11151,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>283</v>
       </c>
@@ -11164,7 +11174,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>283</v>
       </c>
@@ -11187,7 +11197,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>283</v>
       </c>
@@ -11210,7 +11220,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>283</v>
       </c>
@@ -11233,7 +11243,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>283</v>
       </c>
@@ -11256,7 +11266,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>225</v>
       </c>
@@ -11279,7 +11289,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>225</v>
       </c>
@@ -11302,7 +11312,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>225</v>
       </c>
@@ -11325,7 +11335,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>225</v>
       </c>
@@ -11348,7 +11358,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>225</v>
       </c>
@@ -11371,7 +11381,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>225</v>
       </c>
@@ -11394,7 +11404,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>225</v>
       </c>
@@ -11417,7 +11427,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>225</v>
       </c>
@@ -11440,7 +11450,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>326</v>
       </c>
@@ -11463,7 +11473,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>326</v>
       </c>
@@ -11486,7 +11496,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>326</v>
       </c>
@@ -11509,7 +11519,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>326</v>
       </c>
@@ -11532,7 +11542,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>326</v>
       </c>
@@ -11555,7 +11565,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>326</v>
       </c>
@@ -11578,7 +11588,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>326</v>
       </c>
@@ -11601,7 +11611,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>326</v>
       </c>
@@ -11624,7 +11634,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>326</v>
       </c>
@@ -11647,7 +11657,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>326</v>
       </c>
@@ -11670,7 +11680,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>238</v>
       </c>
@@ -11693,7 +11703,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>238</v>
       </c>
@@ -11716,7 +11726,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>238</v>
       </c>
@@ -11739,7 +11749,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>238</v>
       </c>
@@ -11762,7 +11772,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>238</v>
       </c>
@@ -11785,7 +11795,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>238</v>
       </c>
@@ -11808,7 +11818,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>238</v>
       </c>
@@ -11831,7 +11841,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>238</v>
       </c>
@@ -11854,7 +11864,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="278" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>572</v>
       </c>
@@ -11874,7 +11884,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>572</v>
       </c>
@@ -11894,7 +11904,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="280" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>572</v>
       </c>
@@ -11914,7 +11924,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>572</v>
       </c>
@@ -11934,7 +11944,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="282" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>572</v>
       </c>
@@ -11954,7 +11964,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="283" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>572</v>
       </c>
@@ -11977,7 +11987,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>572</v>
       </c>
@@ -12000,7 +12010,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>572</v>
       </c>
@@ -12020,7 +12030,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="286" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>572</v>
       </c>
@@ -12040,7 +12050,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>572</v>
       </c>
@@ -12060,7 +12070,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="288" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>572</v>
       </c>
@@ -12080,7 +12090,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>572</v>
       </c>
@@ -12100,7 +12110,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>335</v>
       </c>
@@ -12123,7 +12133,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>335</v>
       </c>
@@ -12146,7 +12156,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>335</v>
       </c>
@@ -12169,7 +12179,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>335</v>
       </c>
@@ -12193,7 +12203,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H278" xr:uid="{67A4DCC5-5B07-467E-950A-5A2762C3E6F1}"/>
+  <autoFilter ref="A1:H293" xr:uid="{67A4DCC5-5B07-467E-950A-5A2762C3E6F1}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CY"/>
+        <filter val="EE"/>
+        <filter val="LU"/>
+        <filter val="MT"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:J293">
     <sortCondition ref="A2:A293"/>
   </sortState>
@@ -12204,10 +12223,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A65E696-62EA-4ED4-BA1D-03354A87C892}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12223,16 +12242,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1433</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>1434</v>
+        <v>893</v>
       </c>
       <c r="E1" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="F1" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12557,7 +12576,7 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>736</v>
@@ -12617,7 +12636,7 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>736</v>
@@ -12677,7 +12696,7 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>736</v>
@@ -12797,7 +12816,7 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>736</v>
@@ -12817,7 +12836,7 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>736</v>
@@ -13037,7 +13056,7 @@
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>880</v>
@@ -13057,7 +13076,7 @@
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>880</v>
@@ -13077,7 +13096,7 @@
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>880</v>
@@ -13097,7 +13116,7 @@
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>880</v>
@@ -13114,6 +13133,99 @@
       <c r="F45" t="s">
         <v>1142</v>
       </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E46" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
+        <v>732</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E47" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E48" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E49" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E50" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="B51" s="16"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18128,7 +18240,7 @@
   <dimension ref="A2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>